<commit_message>
full dataset corr. saldo moscow
</commit_message>
<xml_diff>
--- a/migforecasting/cities19-21/1/d18.xlsx
+++ b/migforecasting/cities19-21/1/d18.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities19-21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities19-21\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21030" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -1161,29 +1161,29 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,12 +1502,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1524,12 +1524,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1656,22 +1656,22 @@
         <v>37</v>
       </c>
       <c r="B13" s="16">
-        <v>47.6</v>
+        <v>47600</v>
       </c>
       <c r="C13" s="16">
-        <v>1.6</v>
+        <v>1600</v>
       </c>
       <c r="D13" s="17">
-        <v>22.9</v>
+        <v>22900</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1706,22 +1706,22 @@
         <v>6</v>
       </c>
       <c r="B17" s="16">
-        <v>28.9</v>
+        <v>28900</v>
       </c>
       <c r="C17" s="16">
-        <v>96.4</v>
+        <v>96400</v>
       </c>
       <c r="D17" s="17">
-        <v>36.5</v>
+        <v>36500</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
     </row>
     <row r="19" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -2030,12 +2030,12 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="24"/>
     </row>
     <row r="44" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -2102,12 +2102,12 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="25"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
     </row>
     <row r="50" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -2166,12 +2166,12 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="25"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -2188,12 +2188,12 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="25"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
     </row>
     <row r="57" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -2260,12 +2260,12 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="25"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
     </row>
     <row r="63" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -2470,60 +2470,60 @@
       <c r="D79" s="15"/>
     </row>
     <row r="80" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="22" t="s">
+      <c r="A80" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B80" s="22"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
     </row>
     <row r="81" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="22" t="s">
+      <c r="A81" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
     </row>
     <row r="82" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="s">
+      <c r="A82" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="22"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="s">
+      <c r="A83" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="22"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
     </row>
     <row r="84" spans="1:4" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
+      <c r="A84" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="22"/>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
     </row>
     <row r="85" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
+      <c r="A85" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B85" s="22"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
     </row>
     <row r="86" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="22"/>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
     </row>
     <row r="87" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="88" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2534,6 +2534,13 @@
     <row r="93" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A84:D84"/>
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
@@ -2543,13 +2550,6 @@
     <mergeCell ref="A49:D49"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A86:D86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
data corr. (moscow year)
</commit_message>
<xml_diff>
--- a/migforecasting/cities19-21/1/d18.xlsx
+++ b/migforecasting/cities19-21/1/d18.xlsx
@@ -1113,12 +1113,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1161,6 +1155,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1182,8 +1179,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,46 +1502,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="28">
         <v>2019</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="28">
         <v>2020</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="29">
         <v>2021</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>12678.1</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <v>12655.1</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <v>12635.5</v>
       </c>
     </row>
@@ -1549,21 +1549,21 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>1962.3</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="14">
         <v>1979.8</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="15">
         <v>1998.6</v>
       </c>
     </row>
@@ -1571,13 +1571,13 @@
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>821.6</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="14">
         <v>817.5</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="15">
         <v>801.7</v>
       </c>
     </row>
@@ -1585,13 +1585,13 @@
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>7132.8</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <v>7209.6</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="15">
         <v>7305.6</v>
       </c>
     </row>
@@ -1599,13 +1599,13 @@
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <v>3583</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <v>3465.6</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="15">
         <v>3331.3</v>
       </c>
     </row>
@@ -1613,13 +1613,13 @@
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <v>10.7</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="14">
         <v>9.9</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="15">
         <v>10.3</v>
       </c>
     </row>
@@ -1627,13 +1627,13 @@
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <v>9.5</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <v>11.9</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="15">
         <v>13.6</v>
       </c>
     </row>
@@ -1641,13 +1641,13 @@
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <v>1.2</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="14">
         <v>-2</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="15">
         <v>-3.3</v>
       </c>
     </row>
@@ -1655,35 +1655,35 @@
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>47600</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>1600</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="15">
         <v>22900</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="14">
         <v>4898.8</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="14">
         <v>5085.6000000000004</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="15">
         <v>5160.6000000000004</v>
       </c>
     </row>
@@ -1691,13 +1691,13 @@
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="14">
         <v>39.299999999999997</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="14">
         <v>112.6</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="15">
         <v>51.7</v>
       </c>
     </row>
@@ -1705,35 +1705,35 @@
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="14">
         <v>28900</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="14">
         <v>96400</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="15">
         <v>36500</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
     </row>
     <row r="19" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="14">
         <v>100070.2</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="15">
         <v>112768.3</v>
       </c>
     </row>
@@ -1741,13 +1741,13 @@
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="14">
         <v>16935.3</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="15">
         <v>18238.599999999999</v>
       </c>
     </row>
@@ -1755,13 +1755,13 @@
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="16">
         <v>3071</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="17">
         <v>3024</v>
       </c>
     </row>
@@ -1769,13 +1769,13 @@
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="14">
         <v>19.399999999999999</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="14">
         <v>19.600000000000001</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="15">
         <v>22.3</v>
       </c>
     </row>
@@ -1783,13 +1783,13 @@
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="14">
         <v>456.5</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="14">
         <v>452.2</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1797,13 +1797,13 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="14">
         <v>454.8</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="14">
         <v>450</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1811,21 +1811,21 @@
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
     </row>
     <row r="26" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="14">
         <v>77.599999999999994</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="14">
         <v>88.5</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="15">
         <v>92.2</v>
       </c>
     </row>
@@ -1833,13 +1833,13 @@
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="14">
         <v>61.2</v>
       </c>
-      <c r="C27" s="16">
+      <c r="C27" s="14">
         <v>69.900000000000006</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="15">
         <v>72.900000000000006</v>
       </c>
     </row>
@@ -1847,21 +1847,21 @@
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="14">
         <v>106.2</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="14">
         <v>114.3</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="15">
         <v>112.5</v>
       </c>
     </row>
@@ -1869,13 +1869,13 @@
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="14">
         <v>83.8</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="14">
         <v>90.3</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="15">
         <v>89</v>
       </c>
     </row>
@@ -1883,13 +1883,13 @@
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="16">
         <v>149</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="16">
         <v>146</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="17">
         <v>172</v>
       </c>
     </row>
@@ -1897,21 +1897,21 @@
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="14">
         <v>82.6</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="14">
         <v>90.6</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="15">
         <v>80.3</v>
       </c>
     </row>
@@ -1919,13 +1919,13 @@
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="14">
         <v>65.099999999999994</v>
       </c>
-      <c r="C34" s="16">
+      <c r="C34" s="14">
         <v>71.599999999999994</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="15">
         <v>63.5</v>
       </c>
     </row>
@@ -1933,13 +1933,13 @@
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="16">
         <v>2551</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="17">
         <v>1308</v>
       </c>
     </row>
@@ -1947,21 +1947,21 @@
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="14">
         <v>391.8</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="14">
         <v>415</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="15">
         <v>448.1</v>
       </c>
     </row>
@@ -1969,13 +1969,13 @@
       <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="16">
         <v>309</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="16">
         <v>328</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D38" s="17">
         <v>355</v>
       </c>
     </row>
@@ -1983,13 +1983,13 @@
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="16">
         <v>7330202</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="17">
         <v>9276221</v>
       </c>
     </row>
@@ -1997,21 +1997,21 @@
       <c r="A40" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="19"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="16">
         <v>6232571</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="17">
         <v>7690263</v>
       </c>
     </row>
@@ -2019,35 +2019,35 @@
       <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="16">
         <v>1097631</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="17">
         <v>1585958</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="24"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="16">
+      <c r="B44" s="14">
         <v>3268623.2</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="14">
         <v>3839394.4</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="15">
         <v>4839917.7</v>
       </c>
     </row>
@@ -2055,13 +2055,13 @@
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="14">
         <v>23.7</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="14">
         <v>32.1</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="15">
         <v>29</v>
       </c>
     </row>
@@ -2069,21 +2069,21 @@
       <c r="A46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="17"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15"/>
     </row>
     <row r="47" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="16">
+      <c r="B47" s="14">
         <v>5.3</v>
       </c>
-      <c r="C47" s="16">
+      <c r="C47" s="14">
         <v>5.9</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="15">
         <v>5.6</v>
       </c>
     </row>
@@ -2091,35 +2091,35 @@
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="16">
+      <c r="B48" s="14">
         <v>18.399999999999999</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="14">
         <v>26.2</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="15">
         <v>23.3</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="24"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
     </row>
     <row r="50" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C50" s="16">
+      <c r="C50" s="14">
         <v>24473286.300000001</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="15">
         <v>28055590.800000001</v>
       </c>
     </row>
@@ -2127,13 +2127,13 @@
       <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="16">
+      <c r="C51" s="14">
         <v>2610619.6</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="15">
         <v>3744897.2</v>
       </c>
     </row>
@@ -2141,13 +2141,13 @@
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="16">
+      <c r="B52" s="14">
         <v>34</v>
       </c>
-      <c r="C52" s="16">
+      <c r="C52" s="14">
         <v>35.4</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="15">
         <v>35</v>
       </c>
     </row>
@@ -2155,65 +2155,65 @@
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="16">
+      <c r="B53" s="14">
         <v>7.9</v>
       </c>
-      <c r="C53" s="16">
+      <c r="C53" s="14">
         <v>8.9</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="15">
         <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
     </row>
     <row r="55" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="16">
         <v>620458</v>
       </c>
-      <c r="D55" s="19">
+      <c r="D55" s="17">
         <v>569398</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
     </row>
     <row r="57" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="16">
         <v>1090331</v>
       </c>
-      <c r="D58" s="19">
+      <c r="D58" s="17">
         <v>1765556</v>
       </c>
     </row>
@@ -2221,13 +2221,13 @@
       <c r="A59" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C59" s="16">
         <v>7874528</v>
       </c>
-      <c r="D59" s="19">
+      <c r="D59" s="17">
         <v>9823893</v>
       </c>
     </row>
@@ -2235,13 +2235,13 @@
       <c r="A60" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C60" s="16">
         <v>971495</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="17">
         <v>864170</v>
       </c>
     </row>
@@ -2249,35 +2249,35 @@
       <c r="A61" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C61" s="16">
         <v>229494</v>
       </c>
-      <c r="D61" s="19">
+      <c r="D61" s="17">
         <v>233427</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="24"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="23"/>
     </row>
     <row r="63" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="16">
+      <c r="B63" s="14">
         <v>951428</v>
       </c>
-      <c r="C63" s="16">
+      <c r="C63" s="14">
         <v>1094815.1000000001</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="15">
         <v>1358039.1</v>
       </c>
     </row>
@@ -2285,13 +2285,13 @@
       <c r="A64" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="16">
+      <c r="C64" s="14">
         <v>4979.3999999999996</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="15">
         <v>7807.3</v>
       </c>
     </row>
@@ -2299,13 +2299,13 @@
       <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="16">
+      <c r="C65" s="14">
         <v>79564</v>
       </c>
-      <c r="D65" s="17">
+      <c r="D65" s="15">
         <v>128913</v>
       </c>
     </row>
@@ -2313,21 +2313,21 @@
       <c r="A66" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="17"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="15"/>
     </row>
     <row r="67" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B67" s="16">
+      <c r="B67" s="14">
         <v>6.2</v>
       </c>
-      <c r="C67" s="16">
+      <c r="C67" s="14">
         <v>90.3</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D67" s="15">
         <v>118.9</v>
       </c>
     </row>
@@ -2335,13 +2335,13 @@
       <c r="A68" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B68" s="16">
+      <c r="B68" s="14">
         <v>0.7</v>
       </c>
-      <c r="C68" s="16">
+      <c r="C68" s="14">
         <v>1.7</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="15">
         <v>1.9</v>
       </c>
     </row>
@@ -2349,13 +2349,13 @@
       <c r="A69" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C69" s="18">
+      <c r="C69" s="16">
         <v>5357</v>
       </c>
-      <c r="D69" s="19">
+      <c r="D69" s="17">
         <v>6161</v>
       </c>
     </row>
@@ -2363,35 +2363,35 @@
       <c r="A70" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C70" s="18">
+      <c r="C70" s="16">
         <v>6495</v>
       </c>
-      <c r="D70" s="19">
+      <c r="D70" s="17">
         <v>15900</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="11"/>
     </row>
     <row r="72" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="18">
+      <c r="C72" s="16">
         <v>5176492</v>
       </c>
-      <c r="D72" s="19">
+      <c r="D72" s="17">
         <v>6038797</v>
       </c>
     </row>
@@ -2399,13 +2399,13 @@
       <c r="A73" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B73" s="14">
         <v>101.5</v>
       </c>
-      <c r="C73" s="16">
+      <c r="C73" s="14">
         <v>98.1</v>
       </c>
-      <c r="D73" s="17">
+      <c r="D73" s="15">
         <v>109.3</v>
       </c>
     </row>
@@ -2413,117 +2413,117 @@
       <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B74" s="16">
+      <c r="B74" s="14">
         <v>358513</v>
       </c>
-      <c r="C74" s="16">
+      <c r="C74" s="14">
         <v>256364</v>
       </c>
-      <c r="D74" s="17">
+      <c r="D74" s="15">
         <v>374286</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B75" s="20">
+      <c r="B75" s="18">
         <v>103.8</v>
       </c>
-      <c r="C75" s="20">
+      <c r="C75" s="18">
         <v>70.099999999999994</v>
       </c>
-      <c r="D75" s="21">
+      <c r="D75" s="19">
         <v>140.1</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14" t="s">
+      <c r="A76" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+      <c r="A77" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
     </row>
     <row r="78" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
     </row>
     <row r="79" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
     </row>
     <row r="80" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
     </row>
     <row r="81" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="29" t="s">
+      <c r="A81" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B81" s="29"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="29"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
     </row>
     <row r="82" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="29" t="s">
+      <c r="A83" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20"/>
     </row>
     <row r="84" spans="1:4" s="4" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="29" t="s">
+      <c r="A84" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
     </row>
     <row r="85" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
+      <c r="B85" s="20"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="20"/>
     </row>
     <row r="86" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="29" t="s">
+      <c r="A86" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="20"/>
     </row>
     <row r="87" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="88" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2534,13 +2534,6 @@
     <row r="93" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A84:D84"/>
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
@@ -2550,6 +2543,13 @@
     <mergeCell ref="A49:D49"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A84:D84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>